<commit_message>
Adds event template with data
</commit_message>
<xml_diff>
--- a/gbif-ipt-docs/downloads/event_ipt_template_v2.xlsx
+++ b/gbif-ipt-docs/downloads/event_ipt_template_v2.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="1600" yWindow="280" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sample Events" sheetId="2" r:id="rId1"/>
+    <sheet name="Sampling Events" sheetId="2" r:id="rId1"/>
     <sheet name="Associated Occurrences" sheetId="1" r:id="rId2"/>
     <sheet name="README" sheetId="4" r:id="rId3"/>
   </sheets>
@@ -204,6 +204,46 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
+          <t xml:space="preserve">The amount of effort expended during an Event.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Examples:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> "40 trap-nights", "10 observer-hours; 10 km by foot; 30 km by car".</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">RECOMMENDED
+Definition: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
           <t xml:space="preserve">A numeric value for a measurement of the size (time duration, length, area, or volume) of a sample in a sampling event. A sampleSizeValue must have a corresponding sampleSizeUnit.
 </t>
         </r>
@@ -226,7 +266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -266,7 +306,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -306,7 +346,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -346,7 +386,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -386,7 +426,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -426,7 +466,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -466,7 +506,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -506,7 +546,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1171,7 +1211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>occurrenceID</t>
   </si>
@@ -1306,25 +1346,31 @@
     </r>
   </si>
   <si>
-    <t>Sample Event Data</t>
-  </si>
-  <si>
-    <t>Use this template for filling in species data derived from standardized protocols for measuring and observing biodiversity. Upload the template to the IPT where it can be published in Darwin Core Archive (DwC-A) format. Note this template includes two sheets: the Sample Events sheet must be mapped to the Event Core, and the Associated Occurrences must be mapped to the Occurrence Extension (in the IPT).</t>
-  </si>
-  <si>
-    <t>Sample Events</t>
-  </si>
-  <si>
     <t>Associated Occurrences</t>
   </si>
   <si>
     <t>This sheet is used to record the list of sample events indicating what protocol was followed, and information about its sample size and its locality. To enable researchers to infer absence of particular species from events, be sure to include the event even if it has no associated occurrence data. Furthermore, make sure to indicate the "parentEventID" for each event when it is part of an event series.</t>
   </si>
   <si>
-    <t>This sheet is used to record the occurrence data derived from (associated to) each sample event. Each record must link to a sample event via its eventID. Although redundant in some cases, the abundance/cover of the species should be recorded using "individualCount" and the combination of "organismQuantity"/"organismQuantityType". Presence/absence data can be recorded by setting "occurrenceStatus" to "present" or "absent".</t>
-  </si>
-  <si>
     <t>footprintSRS</t>
+  </si>
+  <si>
+    <t>samplingEffort</t>
+  </si>
+  <si>
+    <t>occurrenceStatus</t>
+  </si>
+  <si>
+    <t>Sampling Event Data</t>
+  </si>
+  <si>
+    <t>Use this template for filling in species data derived from standardized protocols for measuring and observing biodiversity. Upload the template to the IPT where it can be published in Darwin Core Archive (DwC-A) format. Note this template includes two sheets: the Sampling Events sheet must be mapped to the Event Core, and the Associated Occurrences must be mapped to the Occurrence Extension (in the IPT).</t>
+  </si>
+  <si>
+    <t>Sampling Events</t>
+  </si>
+  <si>
+    <t>This sheet is used to record the occurrence data derived from (associated to) each sampling event. Each record must link to a sampling event via its eventID. Although redundant in some cases, the abundance/cover of the species should be recorded using "individualCount" and the combination of "organismQuantity"/"organismQuantityType". Presence/absence data can be recorded by setting "occurrenceStatus" to "present" or "absent".</t>
   </si>
 </sst>
 </file>
@@ -1559,9 +1605,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="70">
+  <cellStyleXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1673,7 +1723,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="70">
+  <cellStyles count="74">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1708,6 +1758,8 @@
     <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1742,6 +1794,8 @@
     <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
@@ -2072,10 +2126,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2083,18 +2137,18 @@
     <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="9" width="14.83203125" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.5" customWidth="1"/>
-    <col min="12" max="12" width="16.1640625" customWidth="1"/>
-    <col min="13" max="13" width="13.5" customWidth="1"/>
+    <col min="4" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="10" width="14.83203125" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" customWidth="1"/>
+    <col min="12" max="12" width="16.5" customWidth="1"/>
+    <col min="13" max="13" width="16.1640625" customWidth="1"/>
+    <col min="14" max="14" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2108,30 +2162,33 @@
         <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="J1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2151,8 +2208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2218,7 +2275,7 @@
         <v>12</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2238,7 +2295,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2257,7 +2314,7 @@
     <row r="2" spans="1:2" ht="20">
       <c r="A2" s="18"/>
       <c r="B2" s="11" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2267,7 +2324,7 @@
     <row r="4" spans="1:2" ht="75">
       <c r="A4" s="18"/>
       <c r="B4" s="14" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2284,18 +2341,18 @@
     </row>
     <row r="7" spans="1:2" ht="75">
       <c r="A7" s="12" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="75">
       <c r="A8" s="12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2">

</xml_diff>